<commit_message>
Docker & remote DB is added
</commit_message>
<xml_diff>
--- a/database/Adel.xlsx
+++ b/database/Adel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ranah\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Java Projects\Zalando-Price-Tracker\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31FAAF2-ADD3-4DF9-A387-EEBA3FE4E402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D938F00-ED68-4C1B-AB87-6AC631D1BF82}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B452804C-1F90-44E4-B209-8E503CF47830}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8880" xr2:uid="{B452804C-1F90-44E4-B209-8E503CF47830}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1582,8 +1582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8B872CB-20C7-40F1-8446-F22DD8DAAE6B}">
   <dimension ref="A1:A400"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A387" workbookViewId="0">
-      <selection activeCell="M397" sqref="M397"/>
+    <sheetView tabSelected="1" topLeftCell="A209" workbookViewId="0">
+      <selection activeCell="A218" sqref="A218"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>